<commit_message>
updated to new board revision
</commit_message>
<xml_diff>
--- a/configs/VID-PRO-PTZ/assets/Board/Keys-BoM.xlsx
+++ b/configs/VID-PRO-PTZ/assets/Board/Keys-BoM.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
   <sheets>
-    <sheet sheetId="1" name="BOM_Keys_PCB2_2024-11-08" state="visible" r:id="rId4"/>
+    <sheet sheetId="1" name="BOM_Keys_fixed_PCB2_1_2024-11-0" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
@@ -46,6 +46,30 @@
     <t>1</t>
   </si>
   <si>
+    <t>MX1A-11NW</t>
+  </si>
+  <si>
+    <t>BC1,BC2,BC3,BC4</t>
+  </si>
+  <si>
+    <t>SW-TH_MX1A-11NW</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>CHERRY</t>
+  </si>
+  <si>
+    <t>C3316924</t>
+  </si>
+  <si>
+    <t>LCSC</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
     <t>XY-XH2.54-2A11</t>
   </si>
   <si>
@@ -55,19 +79,13 @@
     <t>HDR-TH_2P-P2.50-V-F-1</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
     <t>XYECONN(辛译)</t>
   </si>
   <si>
     <t>C19271368</t>
   </si>
   <si>
-    <t>LCSC</t>
-  </si>
-  <si>
-    <t>2</t>
+    <t>3</t>
   </si>
   <si>
     <t>WS2812B-B/T</t>
@@ -85,7 +103,7 @@
     <t>C2761795</t>
   </si>
   <si>
-    <t>3</t>
+    <t>4</t>
   </si>
   <si>
     <t>ZX-XH2.54-3PZZ</t>
@@ -101,24 +119,6 @@
   </si>
   <si>
     <t>C7429633</t>
-  </si>
-  <si>
-    <t>4</t>
-  </si>
-  <si>
-    <t>SMD_KEYBOARD-SW</t>
-  </si>
-  <si>
-    <t>U2,U2,U2,U2</t>
-  </si>
-  <si>
-    <t>CPG151101S11-16</t>
-  </si>
-  <si>
-    <t>Kailh(凯华)</t>
-  </si>
-  <si>
-    <t>C5156480</t>
   </si>
 </sst>
 </file>
@@ -605,7 +605,7 @@
         <v>24</v>
       </c>
       <c r="B4">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C4" t="s">
         <v>25</v>
@@ -637,7 +637,7 @@
         <v>30</v>
       </c>
       <c r="B5">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C5" t="s">
         <v>31</v>
@@ -646,13 +646,13 @@
         <v>32</v>
       </c>
       <c r="E5" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="F5" t="s">
         <v>14</v>
       </c>
       <c r="G5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="H5" t="s">
         <v>34</v>

</xml_diff>